<commit_message>
Control for import exposure
</commit_message>
<xml_diff>
--- a/raw_data/eurostat/emp_regions.xlsx
+++ b/raw_data/eurostat/emp_regions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aml/AutoEmp/raw_data/eurostat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7467C2BB-EB99-1242-A95D-9BB47046C492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294A3181-C24D-4547-8980-736B5885E189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10220" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10220" yWindow="-28300" windowWidth="51200" windowHeight="28300" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -44,12 +44,12 @@
     <sheet name="Sheet 27" sheetId="29" r:id="rId29"/>
     <sheet name="Sheet 28" sheetId="30" r:id="rId30"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10075" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10070" uniqueCount="332">
   <si>
     <t>Employment (thousand persons) by NUTS 3 regions [nama_10r_3empers__custom_12429620]</t>
   </si>
@@ -1043,6 +1043,9 @@
   <si>
     <t>total_emp_2000</t>
   </si>
+  <si>
+    <t>total_emp_2012</t>
+  </si>
 </sst>
 </file>
 
@@ -29310,11 +29313,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:G117"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="12" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -29429,25 +29432,25 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>318</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>77</v>
+        <v>324</v>
+      </c>
+      <c r="C12" t="s">
+        <v>331</v>
+      </c>
+      <c r="D12" t="s">
+        <v>325</v>
+      </c>
+      <c r="E12" t="s">
+        <v>326</v>
+      </c>
+      <c r="F12" t="s">
+        <v>327</v>
+      </c>
+      <c r="G12" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -29457,19 +29460,19 @@
       <c r="B13" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="18">
         <v>27139.65</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="18">
         <v>754.82</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="18">
         <v>3005.03</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="18">
         <v>2699.57</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="18">
         <v>1837.78</v>
       </c>
     </row>
@@ -29480,19 +29483,19 @@
       <c r="B14" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="19">
         <v>1929.96</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="19">
         <v>1.1200000000000001</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="19">
         <v>62.76</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="19">
         <v>50.56</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G14" s="19">
         <v>35.42</v>
       </c>
     </row>
@@ -29503,19 +29506,19 @@
       <c r="B15" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="18">
         <v>484.78</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="18">
         <v>5</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="18">
         <v>44.56</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="18">
         <v>39.31</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15" s="18">
         <v>38.18</v>
       </c>
     </row>
@@ -29526,19 +29529,19 @@
       <c r="B16" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="19">
         <v>588.24</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="19">
         <v>2.16</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="19">
         <v>76.89</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="19">
         <v>71.41</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="19">
         <v>41.41</v>
       </c>
     </row>
@@ -29549,19 +29552,19 @@
       <c r="B17" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="18">
         <v>479.37</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="18">
         <v>1.38</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="18">
         <v>39.15</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="18">
         <v>35.17</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="18">
         <v>37.99</v>
       </c>
     </row>
@@ -29572,19 +29575,19 @@
       <c r="B18" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="19">
         <v>1090.77</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="19">
         <v>0.11</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="19">
         <v>88.59</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="19">
         <v>66.39</v>
       </c>
-      <c r="G18" s="15">
+      <c r="G18" s="19">
         <v>42.57</v>
       </c>
     </row>
@@ -29595,19 +29598,19 @@
       <c r="B19" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19" s="18">
         <v>596.88</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="18">
         <v>0.04</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="18">
         <v>42.35</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="18">
         <v>32.19</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19" s="18">
         <v>47.88</v>
       </c>
     </row>
@@ -29618,19 +29621,19 @@
       <c r="B20" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="19">
         <v>573.89</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="19">
         <v>0.24</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E20" s="19">
         <v>31.67</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F20" s="19">
         <v>27.14</v>
       </c>
-      <c r="G20" s="15">
+      <c r="G20" s="19">
         <v>43.28</v>
       </c>
     </row>
@@ -29641,19 +29644,19 @@
       <c r="B21" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C21" s="14">
+      <c r="C21" s="18">
         <v>417.5</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D21" s="18">
         <v>1.24</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="18">
         <v>34.58</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="18">
         <v>31.16</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21" s="18">
         <v>31.26</v>
       </c>
     </row>
@@ -29664,19 +29667,19 @@
       <c r="B22" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C22" s="19">
         <v>113.18</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="19">
         <v>6.18</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="19">
         <v>16.5</v>
       </c>
-      <c r="F22" s="15">
+      <c r="F22" s="19">
         <v>14.83</v>
       </c>
-      <c r="G22" s="15">
+      <c r="G22" s="19">
         <v>7.97</v>
       </c>
     </row>
@@ -29687,19 +29690,19 @@
       <c r="B23" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="18">
         <v>147.97</v>
       </c>
-      <c r="D23" s="14">
+      <c r="D23" s="18">
         <v>5.19</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23" s="18">
         <v>24.3</v>
       </c>
-      <c r="F23" s="14">
+      <c r="F23" s="18">
         <v>22.93</v>
       </c>
-      <c r="G23" s="14">
+      <c r="G23" s="18">
         <v>10.97</v>
       </c>
     </row>
@@ -29710,19 +29713,19 @@
       <c r="B24" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C24" s="15">
+      <c r="C24" s="19">
         <v>85.93</v>
       </c>
-      <c r="D24" s="15">
+      <c r="D24" s="19">
         <v>5.5</v>
       </c>
-      <c r="E24" s="15">
+      <c r="E24" s="19">
         <v>12.56</v>
       </c>
-      <c r="F24" s="15">
+      <c r="F24" s="19">
         <v>11.75</v>
       </c>
-      <c r="G24" s="15">
+      <c r="G24" s="19">
         <v>5.85</v>
       </c>
     </row>
@@ -29733,19 +29736,19 @@
       <c r="B25" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="C25" s="14">
+      <c r="C25" s="18">
         <v>245.95</v>
       </c>
-      <c r="D25" s="14">
+      <c r="D25" s="18">
         <v>7.41</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E25" s="18">
         <v>28.01</v>
       </c>
-      <c r="F25" s="14">
+      <c r="F25" s="18">
         <v>23.35</v>
       </c>
-      <c r="G25" s="14">
+      <c r="G25" s="18">
         <v>18.78</v>
       </c>
     </row>
@@ -29756,19 +29759,19 @@
       <c r="B26" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C26" s="19">
         <v>127.68</v>
       </c>
-      <c r="D26" s="15">
+      <c r="D26" s="19">
         <v>6.3</v>
       </c>
-      <c r="E26" s="15">
+      <c r="E26" s="19">
         <v>20.260000000000002</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F26" s="19">
         <v>18.670000000000002</v>
       </c>
-      <c r="G26" s="15">
+      <c r="G26" s="19">
         <v>9.74</v>
       </c>
     </row>
@@ -29779,19 +29782,19 @@
       <c r="B27" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="C27" s="14">
+      <c r="C27" s="18">
         <v>278.42</v>
       </c>
-      <c r="D27" s="14">
+      <c r="D27" s="18">
         <v>6.69</v>
       </c>
-      <c r="E27" s="14">
+      <c r="E27" s="18">
         <v>39.4</v>
       </c>
-      <c r="F27" s="14">
+      <c r="F27" s="18">
         <v>35.479999999999997</v>
       </c>
-      <c r="G27" s="14">
+      <c r="G27" s="18">
         <v>20.73</v>
       </c>
     </row>
@@ -29802,19 +29805,19 @@
       <c r="B28" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="C28" s="15">
+      <c r="C28" s="19">
         <v>235.35</v>
       </c>
-      <c r="D28" s="15">
+      <c r="D28" s="19">
         <v>10.56</v>
       </c>
-      <c r="E28" s="15">
+      <c r="E28" s="19">
         <v>25.89</v>
       </c>
-      <c r="F28" s="15">
+      <c r="F28" s="19">
         <v>23.46</v>
       </c>
-      <c r="G28" s="15">
+      <c r="G28" s="19">
         <v>16.03</v>
       </c>
     </row>
@@ -29825,19 +29828,19 @@
       <c r="B29" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C29" s="14">
+      <c r="C29" s="18">
         <v>76.900000000000006</v>
       </c>
-      <c r="D29" s="14">
+      <c r="D29" s="18">
         <v>4.96</v>
       </c>
-      <c r="E29" s="14">
+      <c r="E29" s="18">
         <v>9.4</v>
       </c>
-      <c r="F29" s="14">
+      <c r="F29" s="18">
         <v>8.6300000000000008</v>
       </c>
-      <c r="G29" s="14">
+      <c r="G29" s="18">
         <v>5.04</v>
       </c>
     </row>
@@ -29848,19 +29851,19 @@
       <c r="B30" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="C30" s="15">
+      <c r="C30" s="19">
         <v>209.66</v>
       </c>
-      <c r="D30" s="15">
+      <c r="D30" s="19">
         <v>11.33</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30" s="19">
         <v>34.22</v>
       </c>
-      <c r="F30" s="15">
+      <c r="F30" s="19">
         <v>32.270000000000003</v>
       </c>
-      <c r="G30" s="15">
+      <c r="G30" s="19">
         <v>14.66</v>
       </c>
     </row>
@@ -29871,19 +29874,19 @@
       <c r="B31" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="C31" s="14">
+      <c r="C31" s="18">
         <v>124.07</v>
       </c>
-      <c r="D31" s="14">
+      <c r="D31" s="18">
         <v>7.45</v>
       </c>
-      <c r="E31" s="14">
+      <c r="E31" s="18">
         <v>18.55</v>
       </c>
-      <c r="F31" s="14">
+      <c r="F31" s="18">
         <v>17.48</v>
       </c>
-      <c r="G31" s="14">
+      <c r="G31" s="18">
         <v>8.49</v>
       </c>
     </row>
@@ -29894,19 +29897,19 @@
       <c r="B32" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="C32" s="15">
+      <c r="C32" s="19">
         <v>211.81</v>
       </c>
-      <c r="D32" s="15">
+      <c r="D32" s="19">
         <v>5.13</v>
       </c>
-      <c r="E32" s="15">
+      <c r="E32" s="19">
         <v>39.81</v>
       </c>
-      <c r="F32" s="15">
+      <c r="F32" s="19">
         <v>38.270000000000003</v>
       </c>
-      <c r="G32" s="15">
+      <c r="G32" s="19">
         <v>13.26</v>
       </c>
     </row>
@@ -29917,19 +29920,19 @@
       <c r="B33" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="C33" s="14">
+      <c r="C33" s="18">
         <v>94.11</v>
       </c>
-      <c r="D33" s="14">
+      <c r="D33" s="18">
         <v>4.1500000000000004</v>
       </c>
-      <c r="E33" s="14">
+      <c r="E33" s="18">
         <v>18.91</v>
       </c>
-      <c r="F33" s="14">
+      <c r="F33" s="18">
         <v>17.93</v>
       </c>
-      <c r="G33" s="14">
+      <c r="G33" s="18">
         <v>6.89</v>
       </c>
     </row>
@@ -29940,19 +29943,19 @@
       <c r="B34" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="C34" s="15">
+      <c r="C34" s="19">
         <v>75.83</v>
       </c>
-      <c r="D34" s="15">
+      <c r="D34" s="19">
         <v>4.0199999999999996</v>
       </c>
-      <c r="E34" s="15">
+      <c r="E34" s="19">
         <v>14.58</v>
       </c>
-      <c r="F34" s="15">
+      <c r="F34" s="19">
         <v>14.19</v>
       </c>
-      <c r="G34" s="15">
+      <c r="G34" s="19">
         <v>5.37</v>
       </c>
     </row>
@@ -29963,19 +29966,19 @@
       <c r="B35" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="C35" s="14">
+      <c r="C35" s="18">
         <v>53.62</v>
       </c>
-      <c r="D35" s="14">
+      <c r="D35" s="18">
         <v>0.4</v>
       </c>
-      <c r="E35" s="14">
+      <c r="E35" s="18">
         <v>8.3800000000000008</v>
       </c>
-      <c r="F35" s="14">
+      <c r="F35" s="18">
         <v>8.01</v>
       </c>
-      <c r="G35" s="14">
+      <c r="G35" s="18">
         <v>3.07</v>
       </c>
     </row>
@@ -29986,19 +29989,19 @@
       <c r="B36" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="C36" s="15">
+      <c r="C36" s="19">
         <v>280.23</v>
       </c>
-      <c r="D36" s="15">
+      <c r="D36" s="19">
         <v>9.4499999999999993</v>
       </c>
-      <c r="E36" s="15">
+      <c r="E36" s="19">
         <v>31.75</v>
       </c>
-      <c r="F36" s="15">
+      <c r="F36" s="19">
         <v>29.42</v>
       </c>
-      <c r="G36" s="15">
+      <c r="G36" s="19">
         <v>20.12</v>
       </c>
     </row>
@@ -30009,19 +30012,19 @@
       <c r="B37" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="C37" s="14">
+      <c r="C37" s="18">
         <v>189.56</v>
       </c>
-      <c r="D37" s="14">
+      <c r="D37" s="18">
         <v>13.23</v>
       </c>
-      <c r="E37" s="14">
+      <c r="E37" s="18">
         <v>29.53</v>
       </c>
-      <c r="F37" s="14">
+      <c r="F37" s="18">
         <v>27.11</v>
       </c>
-      <c r="G37" s="14">
+      <c r="G37" s="18">
         <v>16.3</v>
       </c>
     </row>
@@ -30032,19 +30035,19 @@
       <c r="B38" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="C38" s="15">
+      <c r="C38" s="19">
         <v>106.77</v>
       </c>
-      <c r="D38" s="15">
+      <c r="D38" s="19">
         <v>8.2200000000000006</v>
       </c>
-      <c r="E38" s="15">
+      <c r="E38" s="19">
         <v>18.86</v>
       </c>
-      <c r="F38" s="15">
+      <c r="F38" s="19">
         <v>18.079999999999998</v>
       </c>
-      <c r="G38" s="15">
+      <c r="G38" s="19">
         <v>8.41</v>
       </c>
     </row>
@@ -30055,19 +30058,19 @@
       <c r="B39" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="C39" s="14">
+      <c r="C39" s="18">
         <v>194.04</v>
       </c>
-      <c r="D39" s="14">
+      <c r="D39" s="18">
         <v>5.72</v>
       </c>
-      <c r="E39" s="14">
+      <c r="E39" s="18">
         <v>35.049999999999997</v>
       </c>
-      <c r="F39" s="14">
+      <c r="F39" s="18">
         <v>33.549999999999997</v>
       </c>
-      <c r="G39" s="14">
+      <c r="G39" s="18">
         <v>15.52</v>
       </c>
     </row>
@@ -30078,19 +30081,19 @@
       <c r="B40" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="C40" s="15">
+      <c r="C40" s="19">
         <v>511.27</v>
       </c>
-      <c r="D40" s="15">
+      <c r="D40" s="19">
         <v>8.6199999999999992</v>
       </c>
-      <c r="E40" s="15">
+      <c r="E40" s="19">
         <v>72.73</v>
       </c>
-      <c r="F40" s="15">
+      <c r="F40" s="19">
         <v>64.680000000000007</v>
       </c>
-      <c r="G40" s="15">
+      <c r="G40" s="19">
         <v>39.04</v>
       </c>
     </row>
@@ -30101,19 +30104,19 @@
       <c r="B41" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C41" s="14">
+      <c r="C41" s="18">
         <v>1027.6600000000001</v>
       </c>
-      <c r="D41" s="14">
+      <c r="D41" s="18">
         <v>13.01</v>
       </c>
-      <c r="E41" s="14">
+      <c r="E41" s="18">
         <v>123.7</v>
       </c>
-      <c r="F41" s="14">
+      <c r="F41" s="18">
         <v>111.65</v>
       </c>
-      <c r="G41" s="14">
+      <c r="G41" s="18">
         <v>62.79</v>
       </c>
     </row>
@@ -30124,19 +30127,19 @@
       <c r="B42" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="C42" s="15">
+      <c r="C42" s="19">
         <v>486.26</v>
       </c>
-      <c r="D42" s="15">
+      <c r="D42" s="19">
         <v>13.42</v>
       </c>
-      <c r="E42" s="15">
+      <c r="E42" s="19">
         <v>64.459999999999994</v>
       </c>
-      <c r="F42" s="15">
+      <c r="F42" s="19">
         <v>58.87</v>
       </c>
-      <c r="G42" s="15">
+      <c r="G42" s="19">
         <v>35.840000000000003</v>
       </c>
     </row>
@@ -30147,19 +30150,19 @@
       <c r="B43" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="C43" s="14">
+      <c r="C43" s="18">
         <v>172.03</v>
       </c>
-      <c r="D43" s="14">
+      <c r="D43" s="18">
         <v>8.5500000000000007</v>
       </c>
-      <c r="E43" s="14">
+      <c r="E43" s="18">
         <v>24.13</v>
       </c>
-      <c r="F43" s="14">
+      <c r="F43" s="18">
         <v>22.43</v>
       </c>
-      <c r="G43" s="14">
+      <c r="G43" s="18">
         <v>12.51</v>
       </c>
     </row>
@@ -30170,19 +30173,19 @@
       <c r="B44" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="C44" s="15">
+      <c r="C44" s="19">
         <v>274.31</v>
       </c>
-      <c r="D44" s="15">
+      <c r="D44" s="19">
         <v>6.14</v>
       </c>
-      <c r="E44" s="15">
+      <c r="E44" s="19">
         <v>42.12</v>
       </c>
-      <c r="F44" s="15">
+      <c r="F44" s="19">
         <v>39.72</v>
       </c>
-      <c r="G44" s="15">
+      <c r="G44" s="19">
         <v>20.260000000000002</v>
       </c>
     </row>
@@ -30193,19 +30196,19 @@
       <c r="B45" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="C45" s="14">
+      <c r="C45" s="18">
         <v>215.49</v>
       </c>
-      <c r="D45" s="14">
+      <c r="D45" s="18">
         <v>9.1</v>
       </c>
-      <c r="E45" s="14">
+      <c r="E45" s="18">
         <v>31.89</v>
       </c>
-      <c r="F45" s="14">
+      <c r="F45" s="18">
         <v>30.27</v>
       </c>
-      <c r="G45" s="14">
+      <c r="G45" s="18">
         <v>12.88</v>
       </c>
     </row>
@@ -30216,19 +30219,19 @@
       <c r="B46" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="C46" s="15">
+      <c r="C46" s="19">
         <v>479.84</v>
       </c>
-      <c r="D46" s="15">
+      <c r="D46" s="19">
         <v>7.66</v>
       </c>
-      <c r="E46" s="15">
+      <c r="E46" s="19">
         <v>71.8</v>
       </c>
-      <c r="F46" s="15">
+      <c r="F46" s="19">
         <v>67.209999999999994</v>
       </c>
-      <c r="G46" s="15">
+      <c r="G46" s="19">
         <v>31.26</v>
       </c>
     </row>
@@ -30239,19 +30242,19 @@
       <c r="B47" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="C47" s="14">
+      <c r="C47" s="18">
         <v>283.17</v>
       </c>
-      <c r="D47" s="14">
+      <c r="D47" s="18">
         <v>6.35</v>
       </c>
-      <c r="E47" s="14">
+      <c r="E47" s="18">
         <v>48.76</v>
       </c>
-      <c r="F47" s="14">
+      <c r="F47" s="18">
         <v>45.09</v>
       </c>
-      <c r="G47" s="14">
+      <c r="G47" s="18">
         <v>20.7</v>
       </c>
     </row>
@@ -30262,19 +30265,19 @@
       <c r="B48" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="C48" s="15">
+      <c r="C48" s="19">
         <v>93.04</v>
       </c>
-      <c r="D48" s="15">
+      <c r="D48" s="19">
         <v>4.51</v>
       </c>
-      <c r="E48" s="15">
+      <c r="E48" s="19">
         <v>17.79</v>
       </c>
-      <c r="F48" s="15">
+      <c r="F48" s="19">
         <v>16.21</v>
       </c>
-      <c r="G48" s="15">
+      <c r="G48" s="19">
         <v>6.41</v>
       </c>
     </row>
@@ -30285,19 +30288,19 @@
       <c r="B49" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="C49" s="14">
+      <c r="C49" s="18">
         <v>116.5</v>
       </c>
-      <c r="D49" s="14">
+      <c r="D49" s="18">
         <v>8.01</v>
       </c>
-      <c r="E49" s="14">
+      <c r="E49" s="18">
         <v>16.72</v>
       </c>
-      <c r="F49" s="14">
+      <c r="F49" s="18">
         <v>14.58</v>
       </c>
-      <c r="G49" s="14">
+      <c r="G49" s="18">
         <v>9.07</v>
       </c>
     </row>
@@ -30308,19 +30311,19 @@
       <c r="B50" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="C50" s="15">
+      <c r="C50" s="19">
         <v>245.39</v>
       </c>
-      <c r="D50" s="15">
+      <c r="D50" s="19">
         <v>19.510000000000002</v>
       </c>
-      <c r="E50" s="15">
+      <c r="E50" s="19">
         <v>28.71</v>
       </c>
-      <c r="F50" s="15">
+      <c r="F50" s="19">
         <v>26.66</v>
       </c>
-      <c r="G50" s="15">
+      <c r="G50" s="19">
         <v>15.2</v>
       </c>
     </row>
@@ -30331,19 +30334,19 @@
       <c r="B51" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="C51" s="14">
+      <c r="C51" s="18">
         <v>71.099999999999994</v>
       </c>
-      <c r="D51" s="14">
+      <c r="D51" s="18">
         <v>3.67</v>
       </c>
-      <c r="E51" s="14">
+      <c r="E51" s="18">
         <v>12.54</v>
       </c>
-      <c r="F51" s="14">
+      <c r="F51" s="18">
         <v>11.9</v>
       </c>
-      <c r="G51" s="14">
+      <c r="G51" s="18">
         <v>4.43</v>
       </c>
     </row>
@@ -30354,19 +30357,19 @@
       <c r="B52" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="C52" s="15">
+      <c r="C52" s="19">
         <v>267.31</v>
       </c>
-      <c r="D52" s="15">
+      <c r="D52" s="19">
         <v>4.29</v>
       </c>
-      <c r="E52" s="15">
+      <c r="E52" s="19">
         <v>27.7</v>
       </c>
-      <c r="F52" s="15">
+      <c r="F52" s="19">
         <v>23.92</v>
       </c>
-      <c r="G52" s="15">
+      <c r="G52" s="19">
         <v>17.47</v>
       </c>
     </row>
@@ -30377,19 +30380,19 @@
       <c r="B53" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="C53" s="14">
+      <c r="C53" s="18">
         <v>63.64</v>
       </c>
-      <c r="D53" s="14">
+      <c r="D53" s="18">
         <v>4.6100000000000003</v>
       </c>
-      <c r="E53" s="14">
+      <c r="E53" s="18">
         <v>9.4</v>
       </c>
-      <c r="F53" s="14">
+      <c r="F53" s="18">
         <v>8.81</v>
       </c>
-      <c r="G53" s="14">
+      <c r="G53" s="18">
         <v>4.47</v>
       </c>
     </row>
@@ -30400,19 +30403,19 @@
       <c r="B54" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C54" s="15">
+      <c r="C54" s="19">
         <v>365.3</v>
       </c>
-      <c r="D54" s="15">
+      <c r="D54" s="19">
         <v>5.4</v>
       </c>
-      <c r="E54" s="15">
+      <c r="E54" s="19">
         <v>52.39</v>
       </c>
-      <c r="F54" s="15">
+      <c r="F54" s="19">
         <v>46.18</v>
       </c>
-      <c r="G54" s="15">
+      <c r="G54" s="19">
         <v>25.33</v>
       </c>
     </row>
@@ -30423,19 +30426,19 @@
       <c r="B55" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="C55" s="14">
+      <c r="C55" s="18">
         <v>135.88999999999999</v>
       </c>
-      <c r="D55" s="14">
+      <c r="D55" s="18">
         <v>4.6500000000000004</v>
       </c>
-      <c r="E55" s="14">
+      <c r="E55" s="18">
         <v>26.02</v>
       </c>
-      <c r="F55" s="14">
+      <c r="F55" s="18">
         <v>24.73</v>
       </c>
-      <c r="G55" s="14">
+      <c r="G55" s="18">
         <v>10.81</v>
       </c>
     </row>
@@ -30446,19 +30449,19 @@
       <c r="B56" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="C56" s="15">
+      <c r="C56" s="19">
         <v>594.47</v>
       </c>
-      <c r="D56" s="15">
+      <c r="D56" s="19">
         <v>13.63</v>
       </c>
-      <c r="E56" s="15">
+      <c r="E56" s="19">
         <v>66.23</v>
       </c>
-      <c r="F56" s="15">
+      <c r="F56" s="19">
         <v>60.49</v>
       </c>
-      <c r="G56" s="15">
+      <c r="G56" s="19">
         <v>43.27</v>
       </c>
     </row>
@@ -30469,19 +30472,19 @@
       <c r="B57" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="C57" s="14">
+      <c r="C57" s="18">
         <v>323.51</v>
       </c>
-      <c r="D57" s="14">
+      <c r="D57" s="18">
         <v>21.19</v>
       </c>
-      <c r="E57" s="14">
+      <c r="E57" s="18">
         <v>49.51</v>
       </c>
-      <c r="F57" s="14">
+      <c r="F57" s="18">
         <v>47.28</v>
       </c>
-      <c r="G57" s="14">
+      <c r="G57" s="18">
         <v>24.07</v>
       </c>
     </row>
@@ -30492,19 +30495,19 @@
       <c r="B58" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="C58" s="15">
+      <c r="C58" s="19">
         <v>123.46</v>
       </c>
-      <c r="D58" s="15">
+      <c r="D58" s="19">
         <v>10.3</v>
       </c>
-      <c r="E58" s="15">
+      <c r="E58" s="19">
         <v>23.28</v>
       </c>
-      <c r="F58" s="15">
+      <c r="F58" s="19">
         <v>22.41</v>
       </c>
-      <c r="G58" s="15">
+      <c r="G58" s="19">
         <v>9.7899999999999991</v>
       </c>
     </row>
@@ -30515,19 +30518,19 @@
       <c r="B59" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="C59" s="14">
+      <c r="C59" s="18">
         <v>218.13</v>
       </c>
-      <c r="D59" s="14">
+      <c r="D59" s="18">
         <v>8.48</v>
       </c>
-      <c r="E59" s="14">
+      <c r="E59" s="18">
         <v>37.72</v>
       </c>
-      <c r="F59" s="14">
+      <c r="F59" s="18">
         <v>36.33</v>
       </c>
-      <c r="G59" s="14">
+      <c r="G59" s="18">
         <v>15.12</v>
       </c>
     </row>
@@ -30538,19 +30541,19 @@
       <c r="B60" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="C60" s="15">
+      <c r="C60" s="19">
         <v>255.04</v>
       </c>
-      <c r="D60" s="15">
+      <c r="D60" s="19">
         <v>14.13</v>
       </c>
-      <c r="E60" s="15">
+      <c r="E60" s="19">
         <v>49.6</v>
       </c>
-      <c r="F60" s="15">
+      <c r="F60" s="19">
         <v>47.89</v>
       </c>
-      <c r="G60" s="15">
+      <c r="G60" s="19">
         <v>24.71</v>
       </c>
     </row>
@@ -30561,19 +30564,19 @@
       <c r="B61" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="C61" s="14">
+      <c r="C61" s="18">
         <v>219.42</v>
       </c>
-      <c r="D61" s="14">
+      <c r="D61" s="18">
         <v>17.91</v>
       </c>
-      <c r="E61" s="14">
+      <c r="E61" s="18">
         <v>26.84</v>
       </c>
-      <c r="F61" s="14">
+      <c r="F61" s="18">
         <v>24.92</v>
       </c>
-      <c r="G61" s="14">
+      <c r="G61" s="18">
         <v>17.57</v>
       </c>
     </row>
@@ -30584,19 +30587,19 @@
       <c r="B62" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="C62" s="15">
+      <c r="C62" s="19">
         <v>356.72</v>
       </c>
-      <c r="D62" s="15">
+      <c r="D62" s="19">
         <v>18.78</v>
       </c>
-      <c r="E62" s="15">
+      <c r="E62" s="19">
         <v>42.34</v>
       </c>
-      <c r="F62" s="15">
+      <c r="F62" s="19">
         <v>39.65</v>
       </c>
-      <c r="G62" s="15">
+      <c r="G62" s="19">
         <v>23.39</v>
       </c>
     </row>
@@ -30607,19 +30610,19 @@
       <c r="B63" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="C63" s="14">
+      <c r="C63" s="18">
         <v>454.95</v>
       </c>
-      <c r="D63" s="14">
+      <c r="D63" s="18">
         <v>15.35</v>
       </c>
-      <c r="E63" s="14">
+      <c r="E63" s="18">
         <v>53.01</v>
       </c>
-      <c r="F63" s="14">
+      <c r="F63" s="18">
         <v>49.3</v>
       </c>
-      <c r="G63" s="14">
+      <c r="G63" s="18">
         <v>31.22</v>
       </c>
     </row>
@@ -30630,19 +30633,19 @@
       <c r="B64" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="C64" s="15">
+      <c r="C64" s="19">
         <v>276.08999999999997</v>
       </c>
-      <c r="D64" s="15">
+      <c r="D64" s="19">
         <v>12.48</v>
       </c>
-      <c r="E64" s="15">
+      <c r="E64" s="19">
         <v>38.15</v>
       </c>
-      <c r="F64" s="15">
+      <c r="F64" s="19">
         <v>36.119999999999997</v>
       </c>
-      <c r="G64" s="15">
+      <c r="G64" s="19">
         <v>23.02</v>
       </c>
     </row>
@@ -30653,19 +30656,19 @@
       <c r="B65" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="C65" s="14">
+      <c r="C65" s="18">
         <v>144.31</v>
       </c>
-      <c r="D65" s="14">
+      <c r="D65" s="18">
         <v>9.44</v>
       </c>
-      <c r="E65" s="14">
+      <c r="E65" s="18">
         <v>16.649999999999999</v>
       </c>
-      <c r="F65" s="14">
+      <c r="F65" s="18">
         <v>14.97</v>
       </c>
-      <c r="G65" s="14">
+      <c r="G65" s="18">
         <v>13.25</v>
       </c>
     </row>
@@ -30676,19 +30679,19 @@
       <c r="B66" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="C66" s="15">
+      <c r="C66" s="19">
         <v>666.37</v>
       </c>
-      <c r="D66" s="15">
+      <c r="D66" s="19">
         <v>32.71</v>
       </c>
-      <c r="E66" s="15">
+      <c r="E66" s="19">
         <v>55.7</v>
       </c>
-      <c r="F66" s="15">
+      <c r="F66" s="19">
         <v>46.48</v>
       </c>
-      <c r="G66" s="15">
+      <c r="G66" s="19">
         <v>46.11</v>
       </c>
     </row>
@@ -30699,19 +30702,19 @@
       <c r="B67" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="C67" s="14">
+      <c r="C67" s="18">
         <v>142.88</v>
       </c>
-      <c r="D67" s="14">
+      <c r="D67" s="18">
         <v>9.0500000000000007</v>
       </c>
-      <c r="E67" s="14">
+      <c r="E67" s="18">
         <v>19.12</v>
       </c>
-      <c r="F67" s="14">
+      <c r="F67" s="18">
         <v>17.61</v>
       </c>
-      <c r="G67" s="14">
+      <c r="G67" s="18">
         <v>11.57</v>
       </c>
     </row>
@@ -30722,19 +30725,19 @@
       <c r="B68" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="C68" s="15">
+      <c r="C68" s="19">
         <v>123.88</v>
       </c>
-      <c r="D68" s="15">
+      <c r="D68" s="19">
         <v>9.7200000000000006</v>
       </c>
-      <c r="E68" s="15">
+      <c r="E68" s="19">
         <v>13.52</v>
       </c>
-      <c r="F68" s="15">
+      <c r="F68" s="19">
         <v>12.21</v>
       </c>
-      <c r="G68" s="15">
+      <c r="G68" s="19">
         <v>9.31</v>
       </c>
     </row>
@@ -30745,19 +30748,19 @@
       <c r="B69" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="C69" s="14">
+      <c r="C69" s="18">
         <v>271.36</v>
       </c>
-      <c r="D69" s="14">
+      <c r="D69" s="18">
         <v>11.09</v>
       </c>
-      <c r="E69" s="14">
+      <c r="E69" s="18">
         <v>30.96</v>
       </c>
-      <c r="F69" s="14">
+      <c r="F69" s="18">
         <v>27.85</v>
       </c>
-      <c r="G69" s="14">
+      <c r="G69" s="18">
         <v>21.22</v>
       </c>
     </row>
@@ -30768,19 +30771,19 @@
       <c r="B70" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="C70" s="15">
+      <c r="C70" s="19">
         <v>95.39</v>
       </c>
-      <c r="D70" s="15">
+      <c r="D70" s="19">
         <v>5.26</v>
       </c>
-      <c r="E70" s="15">
+      <c r="E70" s="19">
         <v>11.98</v>
       </c>
-      <c r="F70" s="15">
+      <c r="F70" s="19">
         <v>10.71</v>
       </c>
-      <c r="G70" s="15">
+      <c r="G70" s="19">
         <v>7.29</v>
       </c>
     </row>
@@ -30791,19 +30794,19 @@
       <c r="B71" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="C71" s="14">
+      <c r="C71" s="18">
         <v>41.44</v>
       </c>
-      <c r="D71" s="14">
+      <c r="D71" s="18">
         <v>5.19</v>
       </c>
-      <c r="E71" s="14">
+      <c r="E71" s="18">
         <v>3.95</v>
       </c>
-      <c r="F71" s="14">
+      <c r="F71" s="18">
         <v>3.72</v>
       </c>
-      <c r="G71" s="14">
+      <c r="G71" s="18">
         <v>2.87</v>
       </c>
     </row>
@@ -30814,19 +30817,19 @@
       <c r="B72" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="C72" s="15">
+      <c r="C72" s="19">
         <v>142.86000000000001</v>
       </c>
-      <c r="D72" s="15">
+      <c r="D72" s="19">
         <v>5.28</v>
       </c>
-      <c r="E72" s="15">
+      <c r="E72" s="19">
         <v>17.02</v>
       </c>
-      <c r="F72" s="15">
+      <c r="F72" s="19">
         <v>15.33</v>
       </c>
-      <c r="G72" s="15">
+      <c r="G72" s="19">
         <v>9.52</v>
       </c>
     </row>
@@ -30837,19 +30840,19 @@
       <c r="B73" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="C73" s="14">
+      <c r="C73" s="18">
         <v>136.78</v>
       </c>
-      <c r="D73" s="14">
+      <c r="D73" s="18">
         <v>9.0500000000000007</v>
       </c>
-      <c r="E73" s="14">
+      <c r="E73" s="18">
         <v>22.42</v>
       </c>
-      <c r="F73" s="14">
+      <c r="F73" s="18">
         <v>20.86</v>
       </c>
-      <c r="G73" s="14">
+      <c r="G73" s="18">
         <v>10.41</v>
       </c>
     </row>
@@ -30860,19 +30863,19 @@
       <c r="B74" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="C74" s="15">
+      <c r="C74" s="19">
         <v>230.96</v>
       </c>
-      <c r="D74" s="15">
+      <c r="D74" s="19">
         <v>15.89</v>
       </c>
-      <c r="E74" s="15">
+      <c r="E74" s="19">
         <v>21.19</v>
       </c>
-      <c r="F74" s="15">
+      <c r="F74" s="19">
         <v>18.59</v>
       </c>
-      <c r="G74" s="15">
+      <c r="G74" s="19">
         <v>18.98</v>
       </c>
     </row>
@@ -30883,19 +30886,19 @@
       <c r="B75" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="C75" s="14">
+      <c r="C75" s="18">
         <v>152.68</v>
       </c>
-      <c r="D75" s="14">
+      <c r="D75" s="18">
         <v>9.7799999999999994</v>
       </c>
-      <c r="E75" s="14">
+      <c r="E75" s="18">
         <v>21.19</v>
       </c>
-      <c r="F75" s="14">
+      <c r="F75" s="18">
         <v>19.77</v>
       </c>
-      <c r="G75" s="14">
+      <c r="G75" s="18">
         <v>11.33</v>
       </c>
     </row>
@@ -30906,19 +30909,19 @@
       <c r="B76" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="C76" s="15">
+      <c r="C76" s="19">
         <v>175.27</v>
       </c>
-      <c r="D76" s="15">
+      <c r="D76" s="19">
         <v>6.56</v>
       </c>
-      <c r="E76" s="15">
+      <c r="E76" s="19">
         <v>20.34</v>
       </c>
-      <c r="F76" s="15">
+      <c r="F76" s="19">
         <v>17.79</v>
       </c>
-      <c r="G76" s="15">
+      <c r="G76" s="19">
         <v>12.23</v>
       </c>
     </row>
@@ -30929,19 +30932,19 @@
       <c r="B77" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="C77" s="14">
+      <c r="C77" s="18">
         <v>124.25</v>
       </c>
-      <c r="D77" s="14">
+      <c r="D77" s="18">
         <v>8.7799999999999994</v>
       </c>
-      <c r="E77" s="14">
+      <c r="E77" s="18">
         <v>7.77</v>
       </c>
-      <c r="F77" s="14">
+      <c r="F77" s="18">
         <v>6.45</v>
       </c>
-      <c r="G77" s="14">
+      <c r="G77" s="18">
         <v>9.3800000000000008</v>
       </c>
     </row>
@@ -30952,19 +30955,19 @@
       <c r="B78" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="C78" s="15">
+      <c r="C78" s="19">
         <v>243.54</v>
       </c>
-      <c r="D78" s="15">
+      <c r="D78" s="19">
         <v>10.09</v>
       </c>
-      <c r="E78" s="15">
+      <c r="E78" s="19">
         <v>23.36</v>
       </c>
-      <c r="F78" s="15">
+      <c r="F78" s="19">
         <v>19.760000000000002</v>
       </c>
-      <c r="G78" s="15">
+      <c r="G78" s="19">
         <v>20.03</v>
       </c>
     </row>
@@ -30975,19 +30978,19 @@
       <c r="B79" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="C79" s="14">
+      <c r="C79" s="18">
         <v>418.79</v>
       </c>
-      <c r="D79" s="14">
+      <c r="D79" s="18">
         <v>9.98</v>
       </c>
-      <c r="E79" s="14">
+      <c r="E79" s="18">
         <v>24.28</v>
       </c>
-      <c r="F79" s="14">
+      <c r="F79" s="18">
         <v>18.98</v>
       </c>
-      <c r="G79" s="14">
+      <c r="G79" s="18">
         <v>30.16</v>
       </c>
     </row>
@@ -30998,19 +31001,19 @@
       <c r="B80" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="C80" s="15">
+      <c r="C80" s="19">
         <v>30.83</v>
       </c>
-      <c r="D80" s="15">
+      <c r="D80" s="19">
         <v>3.23</v>
       </c>
-      <c r="E80" s="15">
+      <c r="E80" s="19">
         <v>2.61</v>
       </c>
-      <c r="F80" s="15">
+      <c r="F80" s="19">
         <v>2.2799999999999998</v>
       </c>
-      <c r="G80" s="15">
+      <c r="G80" s="19">
         <v>2.67</v>
       </c>
     </row>
@@ -31021,19 +31024,19 @@
       <c r="B81" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="C81" s="14">
+      <c r="C81" s="18">
         <v>156.83000000000001</v>
       </c>
-      <c r="D81" s="14">
+      <c r="D81" s="18">
         <v>6.16</v>
       </c>
-      <c r="E81" s="14">
+      <c r="E81" s="18">
         <v>8.49</v>
       </c>
-      <c r="F81" s="14">
+      <c r="F81" s="18">
         <v>7.13</v>
       </c>
-      <c r="G81" s="14">
+      <c r="G81" s="18">
         <v>13.01</v>
       </c>
     </row>
@@ -31044,19 +31047,19 @@
       <c r="B82" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="C82" s="15">
+      <c r="C82" s="19">
         <v>51.95</v>
       </c>
-      <c r="D82" s="15">
+      <c r="D82" s="19">
         <v>2.5299999999999998</v>
       </c>
-      <c r="E82" s="15">
+      <c r="E82" s="19">
         <v>7.04</v>
       </c>
-      <c r="F82" s="15">
+      <c r="F82" s="19">
         <v>5.91</v>
       </c>
-      <c r="G82" s="15">
+      <c r="G82" s="19">
         <v>4.05</v>
       </c>
     </row>
@@ -31067,19 +31070,19 @@
       <c r="B83" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="C83" s="14">
+      <c r="C83" s="18">
         <v>107.99</v>
       </c>
-      <c r="D83" s="14">
+      <c r="D83" s="18">
         <v>11.03</v>
       </c>
-      <c r="E83" s="14">
+      <c r="E83" s="18">
         <v>14.63</v>
       </c>
-      <c r="F83" s="14">
+      <c r="F83" s="18">
         <v>13.29</v>
       </c>
-      <c r="G83" s="14">
+      <c r="G83" s="18">
         <v>9.0500000000000007</v>
       </c>
     </row>
@@ -31090,19 +31093,19 @@
       <c r="B84" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="C84" s="15">
+      <c r="C84" s="19">
         <v>620.04</v>
       </c>
-      <c r="D84" s="15">
+      <c r="D84" s="19">
         <v>6.46</v>
       </c>
-      <c r="E84" s="15">
+      <c r="E84" s="19">
         <v>66.28</v>
       </c>
-      <c r="F84" s="15">
+      <c r="F84" s="19">
         <v>60.69</v>
       </c>
-      <c r="G84" s="15">
+      <c r="G84" s="19">
         <v>41.96</v>
       </c>
     </row>
@@ -31113,19 +31116,19 @@
       <c r="B85" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="C85" s="14">
+      <c r="C85" s="18">
         <v>68.88</v>
       </c>
-      <c r="D85" s="14">
+      <c r="D85" s="18">
         <v>8.92</v>
       </c>
-      <c r="E85" s="14">
+      <c r="E85" s="18">
         <v>6.48</v>
       </c>
-      <c r="F85" s="14">
+      <c r="F85" s="18">
         <v>5.85</v>
       </c>
-      <c r="G85" s="14">
+      <c r="G85" s="18">
         <v>4.99</v>
       </c>
     </row>
@@ -31136,19 +31139,19 @@
       <c r="B86" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="C86" s="8">
+      <c r="C86" s="19">
         <v>63</v>
       </c>
-      <c r="D86" s="15">
+      <c r="D86" s="19">
         <v>5.04</v>
       </c>
-      <c r="E86" s="15">
+      <c r="E86" s="19">
         <v>8.6300000000000008</v>
       </c>
-      <c r="F86" s="15">
+      <c r="F86" s="19">
         <v>7.72</v>
       </c>
-      <c r="G86" s="15">
+      <c r="G86" s="19">
         <v>5.09</v>
       </c>
     </row>
@@ -31159,19 +31162,19 @@
       <c r="B87" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="C87" s="14">
+      <c r="C87" s="18">
         <v>88.04</v>
       </c>
-      <c r="D87" s="14">
+      <c r="D87" s="18">
         <v>3.58</v>
       </c>
-      <c r="E87" s="14">
+      <c r="E87" s="18">
         <v>9.52</v>
       </c>
-      <c r="F87" s="14">
+      <c r="F87" s="18">
         <v>8.52</v>
       </c>
-      <c r="G87" s="14">
+      <c r="G87" s="18">
         <v>6.63</v>
       </c>
     </row>
@@ -31182,19 +31185,19 @@
       <c r="B88" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="C88" s="15">
+      <c r="C88" s="19">
         <v>132.76</v>
       </c>
-      <c r="D88" s="15">
+      <c r="D88" s="19">
         <v>7.4</v>
       </c>
-      <c r="E88" s="15">
+      <c r="E88" s="19">
         <v>16.170000000000002</v>
       </c>
-      <c r="F88" s="15">
+      <c r="F88" s="19">
         <v>14.58</v>
       </c>
-      <c r="G88" s="15">
+      <c r="G88" s="19">
         <v>10.06</v>
       </c>
     </row>
@@ -31205,19 +31208,19 @@
       <c r="B89" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="C89" s="14">
+      <c r="C89" s="18">
         <v>87.02</v>
       </c>
-      <c r="D89" s="14">
+      <c r="D89" s="18">
         <v>6.63</v>
       </c>
-      <c r="E89" s="14">
+      <c r="E89" s="18">
         <v>8.25</v>
       </c>
-      <c r="F89" s="14">
+      <c r="F89" s="18">
         <v>6.58</v>
       </c>
-      <c r="G89" s="14">
+      <c r="G89" s="18">
         <v>6.89</v>
       </c>
     </row>
@@ -31228,19 +31231,19 @@
       <c r="B90" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="C90" s="15">
+      <c r="C90" s="19">
         <v>123.2</v>
       </c>
-      <c r="D90" s="15">
+      <c r="D90" s="19">
         <v>6.83</v>
       </c>
-      <c r="E90" s="15">
+      <c r="E90" s="19">
         <v>17.16</v>
       </c>
-      <c r="F90" s="15">
+      <c r="F90" s="19">
         <v>15.92</v>
       </c>
-      <c r="G90" s="15">
+      <c r="G90" s="19">
         <v>9.18</v>
       </c>
     </row>
@@ -31251,19 +31254,19 @@
       <c r="B91" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="C91" s="14">
+      <c r="C91" s="18">
         <v>57.12</v>
       </c>
-      <c r="D91" s="14">
+      <c r="D91" s="18">
         <v>7.19</v>
       </c>
-      <c r="E91" s="14">
+      <c r="E91" s="18">
         <v>5.37</v>
       </c>
-      <c r="F91" s="14">
+      <c r="F91" s="18">
         <v>4.91</v>
       </c>
-      <c r="G91" s="14">
+      <c r="G91" s="18">
         <v>5.14</v>
       </c>
     </row>
@@ -31274,19 +31277,19 @@
       <c r="B92" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="C92" s="15">
+      <c r="C92" s="19">
         <v>77.87</v>
       </c>
-      <c r="D92" s="15">
+      <c r="D92" s="19">
         <v>5.48</v>
       </c>
-      <c r="E92" s="15">
+      <c r="E92" s="19">
         <v>14.23</v>
       </c>
-      <c r="F92" s="15">
+      <c r="F92" s="19">
         <v>13.44</v>
       </c>
-      <c r="G92" s="15">
+      <c r="G92" s="19">
         <v>6.82</v>
       </c>
     </row>
@@ -31297,19 +31300,19 @@
       <c r="B93" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="C93" s="14">
+      <c r="C93" s="18">
         <v>268.52</v>
       </c>
-      <c r="D93" s="14">
+      <c r="D93" s="18">
         <v>8.1999999999999993</v>
       </c>
-      <c r="E93" s="14">
+      <c r="E93" s="18">
         <v>38.22</v>
       </c>
-      <c r="F93" s="14">
+      <c r="F93" s="18">
         <v>35.4</v>
       </c>
-      <c r="G93" s="14">
+      <c r="G93" s="18">
         <v>17.95</v>
       </c>
     </row>
@@ -31320,19 +31323,19 @@
       <c r="B94" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="C94" s="15">
+      <c r="C94" s="19">
         <v>210.02</v>
       </c>
-      <c r="D94" s="15">
+      <c r="D94" s="19">
         <v>5.9</v>
       </c>
-      <c r="E94" s="15">
+      <c r="E94" s="19">
         <v>42.78</v>
       </c>
-      <c r="F94" s="15">
+      <c r="F94" s="19">
         <v>38.909999999999997</v>
       </c>
-      <c r="G94" s="15">
+      <c r="G94" s="19">
         <v>16.32</v>
       </c>
     </row>
@@ -31343,19 +31346,19 @@
       <c r="B95" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="C95" s="14">
+      <c r="C95" s="18">
         <v>103.12</v>
       </c>
-      <c r="D95" s="14">
+      <c r="D95" s="18">
         <v>4.96</v>
       </c>
-      <c r="E95" s="14">
+      <c r="E95" s="18">
         <v>17.46</v>
       </c>
-      <c r="F95" s="14">
+      <c r="F95" s="18">
         <v>15.54</v>
       </c>
-      <c r="G95" s="14">
+      <c r="G95" s="18">
         <v>9.0399999999999991</v>
       </c>
     </row>
@@ -31366,19 +31369,19 @@
       <c r="B96" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="C96" s="15">
+      <c r="C96" s="19">
         <v>208.83</v>
       </c>
-      <c r="D96" s="15">
+      <c r="D96" s="19">
         <v>9.11</v>
       </c>
-      <c r="E96" s="15">
+      <c r="E96" s="19">
         <v>32.96</v>
       </c>
-      <c r="F96" s="15">
+      <c r="F96" s="19">
         <v>29.22</v>
       </c>
-      <c r="G96" s="15">
+      <c r="G96" s="19">
         <v>16.79</v>
       </c>
     </row>
@@ -31389,19 +31392,19 @@
       <c r="B97" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="C97" s="14">
+      <c r="C97" s="18">
         <v>501.88</v>
       </c>
-      <c r="D97" s="14">
+      <c r="D97" s="18">
         <v>6.5</v>
       </c>
-      <c r="E97" s="14">
+      <c r="E97" s="18">
         <v>75.84</v>
       </c>
-      <c r="F97" s="14">
+      <c r="F97" s="18">
         <v>69.09</v>
       </c>
-      <c r="G97" s="14">
+      <c r="G97" s="18">
         <v>36.67</v>
       </c>
     </row>
@@ -31412,19 +31415,19 @@
       <c r="B98" s="5" t="s">
         <v>277</v>
       </c>
-      <c r="C98" s="15">
+      <c r="C98" s="19">
         <v>285.66000000000003</v>
       </c>
-      <c r="D98" s="15">
+      <c r="D98" s="19">
         <v>6.33</v>
       </c>
-      <c r="E98" s="15">
+      <c r="E98" s="19">
         <v>45.5</v>
       </c>
-      <c r="F98" s="15">
+      <c r="F98" s="19">
         <v>43.25</v>
       </c>
-      <c r="G98" s="15">
+      <c r="G98" s="19">
         <v>22.31</v>
       </c>
     </row>
@@ -31435,19 +31438,19 @@
       <c r="B99" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="C99" s="14">
+      <c r="C99" s="18">
         <v>912.14</v>
       </c>
-      <c r="D99" s="14">
+      <c r="D99" s="18">
         <v>7.7</v>
       </c>
-      <c r="E99" s="14">
+      <c r="E99" s="18">
         <v>99.27</v>
       </c>
-      <c r="F99" s="14">
+      <c r="F99" s="18">
         <v>88.82</v>
       </c>
-      <c r="G99" s="14">
+      <c r="G99" s="18">
         <v>57.44</v>
       </c>
     </row>
@@ -31458,19 +31461,19 @@
       <c r="B100" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="C100" s="15">
+      <c r="C100" s="19">
         <v>201.03</v>
       </c>
-      <c r="D100" s="15">
+      <c r="D100" s="19">
         <v>3.4</v>
       </c>
-      <c r="E100" s="15">
+      <c r="E100" s="19">
         <v>20.57</v>
       </c>
-      <c r="F100" s="15">
+      <c r="F100" s="19">
         <v>17.5</v>
       </c>
-      <c r="G100" s="15">
+      <c r="G100" s="19">
         <v>16.149999999999999</v>
       </c>
     </row>
@@ -31481,19 +31484,19 @@
       <c r="B101" s="5" t="s">
         <v>283</v>
       </c>
-      <c r="C101" s="14">
+      <c r="C101" s="18">
         <v>301.08999999999997</v>
       </c>
-      <c r="D101" s="14">
+      <c r="D101" s="18">
         <v>4.57</v>
       </c>
-      <c r="E101" s="14">
+      <c r="E101" s="18">
         <v>42.72</v>
       </c>
-      <c r="F101" s="14">
+      <c r="F101" s="18">
         <v>40.71</v>
       </c>
-      <c r="G101" s="14">
+      <c r="G101" s="18">
         <v>24.22</v>
       </c>
     </row>
@@ -31504,19 +31507,19 @@
       <c r="B102" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="C102" s="15">
+      <c r="C102" s="19">
         <v>57.61</v>
       </c>
-      <c r="D102" s="15">
+      <c r="D102" s="19">
         <v>2.72</v>
       </c>
-      <c r="E102" s="15">
+      <c r="E102" s="19">
         <v>5.04</v>
       </c>
-      <c r="F102" s="15">
+      <c r="F102" s="19">
         <v>4.2</v>
       </c>
-      <c r="G102" s="15">
+      <c r="G102" s="19">
         <v>4.62</v>
       </c>
     </row>
@@ -31527,19 +31530,19 @@
       <c r="B103" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="C103" s="14">
+      <c r="C103" s="18">
         <v>60.02</v>
       </c>
-      <c r="D103" s="14">
+      <c r="D103" s="18">
         <v>2.3199999999999998</v>
       </c>
-      <c r="E103" s="14">
+      <c r="E103" s="18">
         <v>2.39</v>
       </c>
-      <c r="F103" s="14">
+      <c r="F103" s="18">
         <v>1.74</v>
       </c>
-      <c r="G103" s="14">
+      <c r="G103" s="18">
         <v>5.07</v>
       </c>
     </row>
@@ -31550,19 +31553,19 @@
       <c r="B104" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="C104" s="15">
+      <c r="C104" s="19">
         <v>456.98</v>
       </c>
-      <c r="D104" s="15">
+      <c r="D104" s="19">
         <v>2.4900000000000002</v>
       </c>
-      <c r="E104" s="15">
+      <c r="E104" s="19">
         <v>29.29</v>
       </c>
-      <c r="F104" s="15">
+      <c r="F104" s="19">
         <v>24.59</v>
       </c>
-      <c r="G104" s="15">
+      <c r="G104" s="19">
         <v>32.82</v>
       </c>
     </row>
@@ -31573,19 +31576,19 @@
       <c r="B105" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="C105" s="14">
+      <c r="C105" s="18">
         <v>855.3</v>
       </c>
-      <c r="D105" s="14">
+      <c r="D105" s="18">
         <v>10.27</v>
       </c>
-      <c r="E105" s="14">
+      <c r="E105" s="18">
         <v>72.180000000000007</v>
       </c>
-      <c r="F105" s="14">
+      <c r="F105" s="18">
         <v>60.51</v>
       </c>
-      <c r="G105" s="14">
+      <c r="G105" s="18">
         <v>54.16</v>
       </c>
     </row>
@@ -31596,19 +31599,19 @@
       <c r="B106" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="C106" s="15">
+      <c r="C106" s="19">
         <v>373.84</v>
       </c>
-      <c r="D106" s="8">
+      <c r="D106" s="19">
         <v>8</v>
       </c>
-      <c r="E106" s="15">
+      <c r="E106" s="19">
         <v>20.56</v>
       </c>
-      <c r="F106" s="15">
+      <c r="F106" s="19">
         <v>16.75</v>
       </c>
-      <c r="G106" s="15">
+      <c r="G106" s="19">
         <v>30.12</v>
       </c>
     </row>
@@ -31619,19 +31622,19 @@
       <c r="B107" s="5" t="s">
         <v>295</v>
       </c>
-      <c r="C107" s="14">
+      <c r="C107" s="18">
         <v>225.28</v>
       </c>
-      <c r="D107" s="14">
+      <c r="D107" s="18">
         <v>10.51</v>
       </c>
-      <c r="E107" s="14">
+      <c r="E107" s="18">
         <v>19.5</v>
       </c>
-      <c r="F107" s="14">
+      <c r="F107" s="18">
         <v>16.55</v>
       </c>
-      <c r="G107" s="14">
+      <c r="G107" s="18">
         <v>17.760000000000002</v>
       </c>
     </row>
@@ -31642,19 +31645,19 @@
       <c r="B108" s="5" t="s">
         <v>297</v>
       </c>
-      <c r="C108" s="15">
+      <c r="C108" s="19">
         <v>60.95</v>
       </c>
-      <c r="D108" s="15">
+      <c r="D108" s="19">
         <v>1.39</v>
       </c>
-      <c r="E108" s="15">
+      <c r="E108" s="19">
         <v>3.31</v>
       </c>
-      <c r="F108" s="15">
+      <c r="F108" s="19">
         <v>2.21</v>
       </c>
-      <c r="G108" s="15">
+      <c r="G108" s="19">
         <v>7.64</v>
       </c>
     </row>
@@ -31665,19 +31668,19 @@
       <c r="B109" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="C109" s="14">
+      <c r="C109" s="18">
         <v>59.91</v>
       </c>
-      <c r="D109" s="14">
+      <c r="D109" s="18">
         <v>3.66</v>
       </c>
-      <c r="E109" s="14">
+      <c r="E109" s="18">
         <v>3.04</v>
       </c>
-      <c r="F109" s="14">
+      <c r="F109" s="18">
         <v>2.4700000000000002</v>
       </c>
-      <c r="G109" s="14">
+      <c r="G109" s="18">
         <v>7.46</v>
       </c>
     </row>
@@ -31688,19 +31691,19 @@
       <c r="B110" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="C110" s="15">
+      <c r="C110" s="19">
         <v>128.13</v>
       </c>
-      <c r="D110" s="15">
+      <c r="D110" s="19">
         <v>4.79</v>
       </c>
-      <c r="E110" s="15">
+      <c r="E110" s="19">
         <v>7.94</v>
       </c>
-      <c r="F110" s="15">
+      <c r="F110" s="19">
         <v>6.16</v>
       </c>
-      <c r="G110" s="15">
+      <c r="G110" s="19">
         <v>7.48</v>
       </c>
     </row>
@@ -31711,19 +31714,19 @@
       <c r="B111" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="C111" s="14">
+      <c r="C111" s="18">
         <v>133.62</v>
       </c>
-      <c r="D111" s="14">
+      <c r="D111" s="18">
         <v>8.33</v>
       </c>
-      <c r="E111" s="14">
+      <c r="E111" s="18">
         <v>7.98</v>
       </c>
-      <c r="F111" s="14">
+      <c r="F111" s="18">
         <v>5.92</v>
       </c>
-      <c r="G111" s="14">
+      <c r="G111" s="18">
         <v>7.58</v>
       </c>
     </row>
@@ -31734,19 +31737,19 @@
       <c r="B112" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="C112" s="15">
+      <c r="C112" s="19">
         <v>52.66</v>
       </c>
-      <c r="D112" s="15">
+      <c r="D112" s="19">
         <v>1.33</v>
       </c>
-      <c r="E112" s="15">
+      <c r="E112" s="19">
         <v>3.88</v>
       </c>
-      <c r="F112" s="15">
+      <c r="F112" s="19">
         <v>2.65</v>
       </c>
-      <c r="G112" s="15">
+      <c r="G112" s="19">
         <v>4.05</v>
       </c>
     </row>
@@ -31757,19 +31760,19 @@
       <c r="B113" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="C113" s="14">
+      <c r="C113" s="18">
         <v>264.33999999999997</v>
       </c>
-      <c r="D113" s="14">
+      <c r="D113" s="18">
         <v>11.13</v>
       </c>
-      <c r="E113" s="14">
+      <c r="E113" s="18">
         <v>16.32</v>
       </c>
-      <c r="F113" s="14">
+      <c r="F113" s="18">
         <v>13.47</v>
       </c>
-      <c r="G113" s="14">
+      <c r="G113" s="18">
         <v>17.18</v>
       </c>
     </row>
@@ -31780,21 +31783,11 @@
       <c r="B114" s="5" t="s">
         <v>309</v>
       </c>
-      <c r="C114" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="D114" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="E114" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="F114" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="G114" s="8" t="s">
-        <v>319</v>
-      </c>
+      <c r="C114" s="19"/>
+      <c r="D114" s="19"/>
+      <c r="E114" s="19"/>
+      <c r="F114" s="19"/>
+      <c r="G114" s="19"/>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
@@ -39358,11 +39351,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:G117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="12" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="A12" sqref="A12:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>